<commit_message>
Updated Excel Log Book
Added my hours
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\CSCW\CSCW_Project\Work_Log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alastair\Documents\UVic\Seng435\CSCW_Project\Work_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6240" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -128,13 +128,22 @@
   </si>
   <si>
     <t>Nitin(NG)</t>
+  </si>
+  <si>
+    <t>Read Articles</t>
+  </si>
+  <si>
+    <t>Wrote my part for Proposal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated log book </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,8 +151,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,8 +196,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F8F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -183,18 +217,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -203,14 +246,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A12"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,34 +567,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -571,7 +632,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -586,49 +647,55 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>1.5</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -663,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A12"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,34 +742,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -758,61 +825,74 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
     </row>
   </sheetData>
@@ -827,6 +907,7 @@
     <mergeCell ref="A20:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -834,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,34 +927,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -907,7 +988,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -926,49 +1007,55 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -979,14 +1066,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -996,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,34 +1095,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1087,7 +1174,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -1100,61 +1187,73 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
     </row>
   </sheetData>
@@ -1176,7 +1275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
@@ -1188,34 +1287,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1231,7 +1330,7 @@
       <c r="A10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -1332,34 +1431,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1375,7 +1474,7 @@
       <c r="A10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">

</xml_diff>

<commit_message>
Added more hours to my log
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t xml:space="preserve">Updated log book </t>
+  </si>
+  <si>
+    <t>Added Sql Queries</t>
+  </si>
+  <si>
+    <t>Updated Interview Questions</t>
   </si>
 </sst>
 </file>
@@ -252,15 +258,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -272,6 +269,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,22 +573,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -599,7 +605,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
@@ -610,7 +616,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -619,7 +625,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -628,67 +634,67 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="11"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="11"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="11"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="11"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="11"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="11"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="11"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="11"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="11"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="11"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="A30" s="11"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -699,16 +705,16 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="11"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="A35" s="11"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -742,22 +748,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -774,7 +780,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
@@ -785,7 +791,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -794,7 +800,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -803,7 +809,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="11"/>
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -812,88 +818,88 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="11"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="11"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="11"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="11"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="11"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="11"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="11"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="11"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="11"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="A30" s="11"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="12" t="s">
+      <c r="A33" s="11"/>
+      <c r="B33" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="A35" s="11"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -927,22 +933,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -959,7 +965,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B8" t="s">
@@ -970,7 +976,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -979,7 +985,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -991,58 +997,58 @@
       <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="11"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="11"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="11"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="11"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="11"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="11"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="11"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="11"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="11"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="11"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
@@ -1053,27 +1059,27 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="11"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="11"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="11"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A30:A34"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A30:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1084,7 +1090,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,22 +1101,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1127,7 +1133,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
@@ -1138,7 +1144,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -1147,7 +1153,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -1156,7 +1162,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="11"/>
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -1165,7 +1171,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="11"/>
       <c r="B12" t="s">
         <v>31</v>
       </c>
@@ -1177,58 +1183,58 @@
       <c r="A13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="11"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="11"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="11"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="11"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="11"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="11"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="11"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="11"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="11"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="A30" s="11"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -1239,7 +1245,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="11"/>
       <c r="B33" t="s">
         <v>35</v>
       </c>
@@ -1248,13 +1254,25 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="A35" s="11"/>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1287,22 +1305,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1319,86 +1337,86 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="11"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="11"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="11"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="11"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="11"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="11"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="11"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="11"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="11"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="11"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="11"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="11"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="11"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1431,22 +1449,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1463,86 +1481,86 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="11"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="11"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="11"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="11"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="11"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="11"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="11"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="11"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="11"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="11"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="11"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="11"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="11"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Updated Log and added more test scripts
- Updated Log
- Added tor test script to start fixing rate limiting issue with data
extractor
- Added stub for README.md which will contain install instructions when
finished
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alastair\Documents\UVic\Seng435\CSCW_Project\Work_Log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/breckwagner/github/CSCW_Project/Work_Log/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6240" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27560" windowHeight="16140" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,12 @@
     <sheet name="Week 5" sheetId="5" r:id="rId5"/>
     <sheet name="Week 6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -143,6 +146,18 @@
   </si>
   <si>
     <t>Updated Interview Questions</t>
+  </si>
+  <si>
+    <t>Email Template (2015-10-24)</t>
+  </si>
+  <si>
+    <t>StackOverflow/Github/Twitter API Research (2015-10-24)</t>
+  </si>
+  <si>
+    <t>Web Scraper Python Script (2015-10-24)</t>
+  </si>
+  <si>
+    <t>Thursday Meeting on Survey Questions (2015-10-22)</t>
   </si>
 </sst>
 </file>
@@ -342,9 +357,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -377,9 +392,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -565,38 +580,38 @@
       <selection activeCell="B32" sqref="B32:C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -604,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
@@ -615,7 +630,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>5</v>
@@ -624,7 +639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>6</v>
@@ -633,67 +648,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
@@ -704,16 +719,16 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
     </row>
   </sheetData>
@@ -736,42 +751,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -779,7 +794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
@@ -790,7 +805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>9</v>
@@ -799,7 +814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>10</v>
@@ -808,7 +823,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" t="s">
         <v>11</v>
@@ -817,62 +832,62 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
@@ -883,7 +898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="9" t="s">
         <v>34</v>
@@ -892,13 +907,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
     </row>
   </sheetData>
@@ -921,42 +936,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -964,7 +979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -975,7 +990,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>13</v>
@@ -984,7 +999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>14</v>
@@ -993,61 +1008,61 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
@@ -1058,16 +1073,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
     </row>
   </sheetData>
@@ -1089,42 +1104,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1132,7 +1147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
@@ -1143,7 +1158,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>16</v>
@@ -1152,7 +1167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>17</v>
@@ -1161,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" t="s">
         <v>18</v>
@@ -1170,7 +1185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" t="s">
         <v>31</v>
@@ -1179,61 +1194,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
@@ -1244,7 +1283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" t="s">
         <v>35</v>
@@ -1253,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" t="s">
         <v>36</v>
@@ -1262,7 +1301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" t="s">
         <v>37</v>
@@ -1271,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
     </row>
   </sheetData>
@@ -1297,38 +1336,38 @@
       <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1336,86 +1375,86 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
     </row>
   </sheetData>
@@ -1441,38 +1480,38 @@
       <selection activeCell="A12" sqref="A12:A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1480,86 +1519,86 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Log + Removed log_breckwagner.md
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27560" windowHeight="16140" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15760" windowHeight="15300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="44">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Thursday Meeting on Survey Questions (2015-10-22)</t>
+  </si>
+  <si>
+    <t>Project Reading/Contributions to Proposal</t>
+  </si>
+  <si>
+    <t>Project Meeting</t>
   </si>
 </sst>
 </file>
@@ -576,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -677,6 +683,12 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>1.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -751,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -856,9 +868,21 @@
       <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
@@ -936,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1104,7 +1128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Pushing Ethics application, consent form, Interview questions, Survey and my Work_log(updated)
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/breckwagner/github/CSCW_Project/Work_Log/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\CSCW\CSCW_Project\Work_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15760" windowHeight="15300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="15765" windowHeight="15300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,11 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -88,9 +88,6 @@
     <t>Interview Questions design with Arturo</t>
   </si>
   <si>
-    <t>Complete Ethics application</t>
-  </si>
-  <si>
     <t>Week 1 (28th Sept – 2nd October)</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>Project Meeting</t>
+  </si>
+  <si>
+    <t>Complete Ethics application, with the feedback</t>
   </si>
 </sst>
 </file>
@@ -582,42 +582,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -625,9 +625,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -636,7 +636,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>5</v>
@@ -645,7 +645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>6</v>
@@ -654,35 +654,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -691,38 +691,38 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
@@ -731,16 +731,16 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
     </row>
   </sheetData>
@@ -763,42 +763,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -806,9 +806,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -817,7 +817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>9</v>
@@ -826,7 +826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>10</v>
@@ -835,7 +835,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" t="s">
         <v>11</v>
@@ -844,100 +844,100 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-    </row>
-    <row r="31" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>30</v>
-      </c>
       <c r="B32" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
     </row>
   </sheetData>
@@ -960,42 +960,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1003,9 +1003,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -1014,7 +1014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>13</v>
@@ -1023,7 +1023,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>14</v>
@@ -1032,63 +1032,63 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
@@ -1097,16 +1097,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
     </row>
   </sheetData>
@@ -1128,42 +1128,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1171,9 +1171,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -1182,7 +1182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>16</v>
@@ -1191,7 +1191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>17</v>
@@ -1200,105 +1200,105 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>2.5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
@@ -1307,34 +1307,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
     </row>
   </sheetData>
@@ -1360,38 +1360,38 @@
       <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1399,86 +1399,86 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
     </row>
   </sheetData>
@@ -1504,38 +1504,38 @@
       <selection activeCell="A12" sqref="A12:A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1543,86 +1543,86 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit Project Diary xlsx
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alastair\Documents\UVic\Seng435\CSCW_Project\Work_Log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arturo\Documents\CollaborativeWork\Project\CSCW_Project\Work_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6240" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,23 @@
     <sheet name="Week 5" sheetId="5" r:id="rId5"/>
     <sheet name="Week 6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -85,9 +91,6 @@
     <t>Interview Questions design with Arturo</t>
   </si>
   <si>
-    <t>Complete Ethics application</t>
-  </si>
-  <si>
     <t>Week 1 (28th Sept – 2nd October)</t>
   </si>
   <si>
@@ -137,6 +140,81 @@
   </si>
   <si>
     <t xml:space="preserve">Updated log book </t>
+  </si>
+  <si>
+    <t>Added Sql Queries</t>
+  </si>
+  <si>
+    <t>Updated Interview Questions</t>
+  </si>
+  <si>
+    <t>Email Template (2015-10-24)</t>
+  </si>
+  <si>
+    <t>StackOverflow/Github/Twitter API Research (2015-10-24)</t>
+  </si>
+  <si>
+    <t>Web Scraper Python Script (2015-10-24)</t>
+  </si>
+  <si>
+    <t>Thursday Meeting on Survey Questions (2015-10-22)</t>
+  </si>
+  <si>
+    <t>Project Reading/Contributions to Proposal</t>
+  </si>
+  <si>
+    <t>Project Meeting</t>
+  </si>
+  <si>
+    <t>Complete Ethics application, with the feedback</t>
+  </si>
+  <si>
+    <t>Meeting with Nitin: Discuss about Literature review and Project Ideas</t>
+  </si>
+  <si>
+    <t>Research for new Literature Review about our final idea: How to improve collaboration through Gamification in Stack Overflow?</t>
+  </si>
+  <si>
+    <t>Group meeting: Define final project idea, literature review papers to be assigned to team members.</t>
+  </si>
+  <si>
+    <t>Read research papers and write the work Related section.</t>
+  </si>
+  <si>
+    <t>Literature Review for Initial Idea: Slack</t>
+  </si>
+  <si>
+    <t>Articulation Work: Create a shared Repository and calendar</t>
+  </si>
+  <si>
+    <t>First Brainstorm Meeting</t>
+  </si>
+  <si>
+    <t>Read researches related to Gamification, StackOverflow and qualitative methods</t>
+  </si>
+  <si>
+    <t>Write the final proposal: Methodology, Research Questions and Literature Review</t>
+  </si>
+  <si>
+    <t>Revise all sections of the final proposal. Define the milestones, activities and roles</t>
+  </si>
+  <si>
+    <t>Fill out partially the Ethics application form</t>
+  </si>
+  <si>
+    <t>Create Google forms for survey and interview including some questions to facilitate meeting</t>
+  </si>
+  <si>
+    <t>Friday meeting to complete survey questions and check activities and responsibilities by member on the project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thursday survey question meeting </t>
+  </si>
+  <si>
+    <t>Meeting with Nitin to include more interview questions</t>
+  </si>
+  <si>
+    <t>Modify Milestones according to feedback and including more detail activities</t>
   </si>
 </sst>
 </file>
@@ -236,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -252,15 +330,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -273,12 +342,53 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -336,9 +446,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -371,9 +481,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -555,11 +665,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:C32"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
@@ -567,27 +677,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9"/>
+      <c r="B2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -599,8 +709,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>26</v>
+      <c r="A8" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -610,7 +720,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -619,7 +729,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -628,68 +738,92 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="11"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
@@ -699,16 +833,16 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="11"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="A35" s="11"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -730,11 +864,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
@@ -742,27 +876,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9"/>
+      <c r="B2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -774,8 +908,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>26</v>
+      <c r="A8" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -785,7 +919,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -794,7 +928,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -803,7 +937,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="11"/>
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -812,88 +946,124 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="11"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="11"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="11"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="A30" s="11"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="10" t="s">
+      <c r="A32" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C33" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="13">
-        <v>2</v>
-      </c>
-    </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="A35" s="11"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -915,11 +1085,203 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A12:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
@@ -927,27 +1289,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9"/>
+      <c r="B2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -959,315 +1321,223 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>32</v>
+      <c r="A8" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" s="11"/>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A30:A34"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A33:A37"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A14:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1276,10 +1546,10 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A10"/>
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
@@ -1287,27 +1557,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9"/>
+      <c r="B2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1319,86 +1589,86 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>26</v>
+      <c r="A8" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="11"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="11"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="11"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1419,11 +1689,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
@@ -1431,27 +1701,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9"/>
+      <c r="B2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1463,86 +1733,86 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>21</v>
+      <c r="A8" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="11"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="11"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="11"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Removed old Log and Updated new
Removed my old log file and have updated the new excel log with my hours
worked
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alastair\Documents\UVic\Seng435\CSCW_Project\Work_Log\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6240" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6240" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
     <sheet name="Week 5" sheetId="5" r:id="rId5"/>
     <sheet name="Week 6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -143,6 +138,24 @@
   </si>
   <si>
     <t>Added Sql Queries and results</t>
+  </si>
+  <si>
+    <t>Wrote the intro for Proposal</t>
+  </si>
+  <si>
+    <t>Project Brainstorm Meeting</t>
+  </si>
+  <si>
+    <t>Updating log book</t>
+  </si>
+  <si>
+    <t>Survey question creation meeting (Telecommute from class)</t>
+  </si>
+  <si>
+    <t>Friday meeting to complete survey questions and Milestone confirmation</t>
+  </si>
+  <si>
+    <t>Improving my portion of the proposal based on feedback</t>
   </si>
 </sst>
 </file>
@@ -339,7 +352,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -374,7 +387,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -551,7 +564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:C32"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,6 +692,12 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26">
+        <v>1.5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -736,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,9 +877,21 @@
       <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
@@ -921,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -1033,6 +1064,12 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,12 +1257,30 @@
       <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
@@ -1293,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,49 +1422,55 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updating Milestones and Work_log
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arturo\Documents\CollaborativeWork\Project\CSCW_Project\Work_Log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\CSCW\CSCW_Project\Work_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -230,6 +230,15 @@
   </si>
   <si>
     <t>Improving my portion of the proposal based on feedback</t>
+  </si>
+  <si>
+    <t>Friday Meeting</t>
+  </si>
+  <si>
+    <t>Improve the survey Template based on pilot</t>
+  </si>
+  <si>
+    <t>Updated Milestones,Improving Email template for Survey, Sending emails to participants</t>
   </si>
 </sst>
 </file>
@@ -685,11 +694,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
@@ -890,11 +899,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B26" sqref="B26:C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
@@ -1123,11 +1132,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="93.140625" customWidth="1"/>
@@ -1321,11 +1330,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
@@ -1607,11 +1616,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
@@ -1654,12 +1663,30 @@
       <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -1761,7 +1788,7 @@
       <selection activeCell="A12" sqref="A12:A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Updated work log with hours for week 5/6
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arturo\Documents\CollaborativeWork\Project\CSCW_Project\Work_Log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/breckwagner/github/CSCW_Project/Work_Log/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24980" windowHeight="13560" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -254,6 +257,18 @@
   </si>
   <si>
     <t>Improve the survey according to pilot. Send emails to 300 users and plan the organization of data collection.</t>
+  </si>
+  <si>
+    <t>Huge amount of work improving the data extractor program</t>
+  </si>
+  <si>
+    <t>Week 5 (31th Oct – 6th November)</t>
+  </si>
+  <si>
+    <t>Compiling output of "data_extractor.py"</t>
+  </si>
+  <si>
+    <t>Compiling output of "data_extractor.py" for high/medium/random groups (low group failed to work)</t>
   </si>
 </sst>
 </file>
@@ -713,38 +728,38 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -752,7 +767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
@@ -763,7 +778,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>5</v>
@@ -772,7 +787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>6</v>
@@ -781,16 +796,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>26</v>
       </c>
@@ -801,7 +816,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" t="s">
         <v>49</v>
@@ -810,7 +825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" t="s">
         <v>48</v>
@@ -819,13 +834,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
@@ -836,19 +851,19 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -859,19 +874,19 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>29</v>
       </c>
@@ -882,16 +897,16 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
     </row>
   </sheetData>
@@ -918,38 +933,38 @@
       <selection activeCell="B26" sqref="B26:C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -957,7 +972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
@@ -968,7 +983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>9</v>
@@ -977,7 +992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>10</v>
@@ -986,7 +1001,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
       <c r="B11" t="s">
         <v>11</v>
@@ -995,10 +1010,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>26</v>
       </c>
@@ -1009,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="11" t="s">
         <v>45</v>
@@ -1018,7 +1033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" t="s">
         <v>46</v>
@@ -1027,7 +1042,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" t="s">
         <v>47</v>
@@ -1036,10 +1051,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
@@ -1050,7 +1065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" t="s">
         <v>42</v>
@@ -1059,16 +1074,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -1079,7 +1094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="13" t="s">
         <v>61</v>
@@ -1088,17 +1103,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>29</v>
       </c>
@@ -1109,7 +1124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="9" t="s">
         <v>33</v>
@@ -1118,13 +1133,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
     </row>
   </sheetData>
@@ -1151,38 +1166,38 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1190,7 +1205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>31</v>
       </c>
@@ -1201,7 +1216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>13</v>
@@ -1210,7 +1225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>14</v>
@@ -1219,10 +1234,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -1233,7 +1248,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" t="s">
         <v>51</v>
@@ -1242,7 +1257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" t="s">
         <v>52</v>
@@ -1251,7 +1266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" t="s">
         <v>53</v>
@@ -1260,27 +1275,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>28</v>
       </c>
@@ -1291,19 +1306,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>29</v>
       </c>
@@ -1314,16 +1329,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
     </row>
   </sheetData>
@@ -1349,38 +1364,38 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1388,7 +1403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
@@ -1399,7 +1414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>16</v>
@@ -1408,7 +1423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>17</v>
@@ -1417,7 +1432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
       <c r="B11" t="s">
         <v>43</v>
@@ -1426,7 +1441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
       <c r="B12" t="s">
         <v>30</v>
@@ -1435,10 +1450,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>26</v>
       </c>
@@ -1449,7 +1464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" t="s">
         <v>55</v>
@@ -1458,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" t="s">
         <v>57</v>
@@ -1467,7 +1482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" t="s">
         <v>56</v>
@@ -1476,7 +1491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" t="s">
         <v>58</v>
@@ -1485,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" t="s">
         <v>59</v>
@@ -1494,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>27</v>
       </c>
@@ -1505,7 +1520,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" t="s">
         <v>37</v>
@@ -1514,7 +1529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" t="s">
         <v>38</v>
@@ -1523,7 +1538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" t="s">
         <v>39</v>
@@ -1532,10 +1547,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>28</v>
       </c>
@@ -1546,7 +1561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="15" t="s">
         <v>63</v>
@@ -1555,7 +1570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="15" t="s">
         <v>64</v>
@@ -1564,13 +1579,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>29</v>
       </c>
@@ -1581,7 +1596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" t="s">
         <v>34</v>
@@ -1590,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" t="s">
         <v>35</v>
@@ -1599,7 +1614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" t="s">
         <v>36</v>
@@ -1608,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
     </row>
   </sheetData>
@@ -1632,41 +1647,41 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1674,7 +1689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
@@ -1685,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>67</v>
@@ -1694,7 +1709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>68</v>
@@ -1703,10 +1718,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -1717,7 +1732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="16" t="s">
         <v>70</v>
@@ -1726,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="16" t="s">
         <v>71</v>
@@ -1735,7 +1750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="16" t="s">
         <v>72</v>
@@ -1744,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="16" t="s">
         <v>73</v>
@@ -1753,24 +1768,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>28</v>
       </c>
@@ -1781,33 +1811,33 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
     </row>
   </sheetData>
@@ -1830,41 +1860,41 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A34"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1872,86 +1902,89 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating my work logs
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\CSCW\CSCW_Project\Work_Log\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760" activeTab="6"/>
   </bookViews>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="102">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -332,6 +337,12 @@
   </si>
   <si>
     <t>Worked on interim report</t>
+  </si>
+  <si>
+    <t>Conducted interview with arturo</t>
+  </si>
+  <si>
+    <t>Created Interim report in collaboration with Arturo</t>
   </si>
 </sst>
 </file>
@@ -777,7 +788,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2206,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,9 +2265,21 @@
       <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
+      <c r="B8" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
+      <c r="B9" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="16">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>

</xml_diff>

<commit_message>
updating missing items to the work log
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="103">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>Created Interim report in collaboration with Arturo</t>
+  </si>
+  <si>
+    <t>Friday Meeting to finalise the changes in the report</t>
   </si>
 </sst>
 </file>
@@ -2217,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,11 +2281,17 @@
         <v>101</v>
       </c>
       <c r="C9" s="16">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
+      <c r="B10" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>

</xml_diff>

<commit_message>
Updating work Log for this week
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\CSCW\CSCW_Project\Work_Log\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -15,6 +20,7 @@
     <sheet name="Week 6" sheetId="6" r:id="rId6"/>
     <sheet name="Week 7" sheetId="8" r:id="rId7"/>
     <sheet name="Week8" sheetId="9" r:id="rId8"/>
+    <sheet name="Week9" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="6" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="116">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -257,9 +263,6 @@
     <t>Huge amount of work improving the data extractor program</t>
   </si>
   <si>
-    <t>Week 5 (31th Oct – 6th November)</t>
-  </si>
-  <si>
     <t>Compiling output of "data_extractor.py" for high/medium/random groups (low group failed to work)</t>
   </si>
   <si>
@@ -317,9 +320,6 @@
     <t>Progress Presentation</t>
   </si>
   <si>
-    <t>Week 5 (7th Nov – 13th November)</t>
-  </si>
-  <si>
     <t>Conducted Interviews</t>
   </si>
   <si>
@@ -356,9 +356,6 @@
     <t>Friday meeting to give format to changes in report</t>
   </si>
   <si>
-    <t>Week 5 (16th Nov – 20th November)</t>
-  </si>
-  <si>
     <t>Last Interview with StackOverflow member</t>
   </si>
   <si>
@@ -372,6 +369,24 @@
   </si>
   <si>
     <t xml:space="preserve">Meeting with Peggy </t>
+  </si>
+  <si>
+    <t>Week 6(31th Oct – 6th November)</t>
+  </si>
+  <si>
+    <t>Week 7 (7th Nov – 13th November)</t>
+  </si>
+  <si>
+    <t>Week 8 (16th Nov – 20th November)</t>
+  </si>
+  <si>
+    <t>Week 9 (23th Nov – 27th November)</t>
+  </si>
+  <si>
+    <t>Report contribution(Abstract, Methodology,General typos and grammar correction)</t>
+  </si>
+  <si>
+    <t>Transcribed interview</t>
   </si>
 </sst>
 </file>
@@ -817,7 +832,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1865,7 +1880,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="16">
         <v>2</v>
@@ -1882,7 +1897,7 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -1917,7 +1932,7 @@
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1926,7 +1941,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1958,7 +1973,7 @@
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1993,7 +2008,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,7 +2039,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2040,7 +2055,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2049,7 +2064,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2067,7 +2082,7 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2081,7 +2096,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="16">
         <v>1.5</v>
@@ -2090,7 +2105,7 @@
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="16">
         <v>1</v>
@@ -2099,7 +2114,7 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="16">
         <v>3</v>
@@ -2108,7 +2123,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="16">
         <v>2</v>
@@ -2117,7 +2132,7 @@
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="16">
         <v>1</v>
@@ -2126,7 +2141,7 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="16">
         <v>1</v>
@@ -2138,7 +2153,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -2161,7 +2176,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26">
         <v>1.5</v>
@@ -2179,7 +2194,7 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2205,7 +2220,7 @@
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2214,7 +2229,7 @@
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34">
         <v>1.5</v>
@@ -2246,8 +2261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,7 +2294,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2295,7 +2310,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C8" s="16">
         <v>2</v>
@@ -2304,7 +2319,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C9" s="16">
         <v>10</v>
@@ -2313,7 +2328,7 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C10" s="16">
         <v>2</v>
@@ -2330,7 +2345,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C13" s="16">
         <v>2</v>
@@ -2339,7 +2354,7 @@
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C14" s="16">
         <v>2.5</v>
@@ -2348,7 +2363,7 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" s="16">
         <v>10</v>
@@ -2357,7 +2372,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C16" s="16">
         <v>2</v>
@@ -2391,7 +2406,7 @@
         <v>28</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C26" s="16">
         <v>0.5</v>
@@ -2400,7 +2415,7 @@
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C27" s="16">
         <v>7</v>
@@ -2409,7 +2424,7 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" s="16">
         <v>1</v>
@@ -2418,7 +2433,7 @@
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C29" s="16">
         <v>1.5</v>
@@ -2432,7 +2447,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C32" s="16">
         <v>7</v>
@@ -2441,7 +2456,7 @@
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C33" s="16">
         <v>1</v>
@@ -2476,8 +2491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,7 +2536,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C6" s="16"/>
     </row>
@@ -2539,7 +2554,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C8" s="16">
         <v>2</v>
@@ -2548,7 +2563,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -2566,7 +2581,7 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C11" s="16">
         <v>1</v>
@@ -2582,7 +2597,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C13" s="16">
         <v>2</v>
@@ -2591,7 +2606,7 @@
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2609,7 +2624,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C16" s="16">
         <v>2</v>
@@ -2667,7 +2682,7 @@
         <v>28</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C26" s="16">
         <v>1</v>
@@ -2676,7 +2691,7 @@
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C27" s="16">
         <v>1</v>
@@ -2705,7 +2720,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C32" s="16">
         <v>7</v>
@@ -2714,7 +2729,7 @@
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C33" s="16">
         <v>1</v>
@@ -2734,6 +2749,202 @@
       <c r="A36" s="17"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A20:A24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="99.42578125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="19"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="19"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="C11" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Adding deliverables and worklog(NG,AR,RBW)
</commit_message>
<xml_diff>
--- a/Work_Log/Team_Project Diary.xlsx
+++ b/Work_Log/Team_Project Diary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/breckwagner/github/CSCW_Project/Work_Log/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\CSCW\CSCW_Project\Work_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Week 7" sheetId="8" r:id="rId7"/>
     <sheet name="Week8" sheetId="9" r:id="rId8"/>
     <sheet name="Week9" sheetId="10" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="6" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -28,18 +29,18 @@
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
   <si>
     <t>Project Diary (Log Book)</t>
   </si>
@@ -426,12 +427,21 @@
   </si>
   <si>
     <t>Meeting (2015-11-27)</t>
+  </si>
+  <si>
+    <t>Week 9 (30th Nov – 4th November)</t>
+  </si>
+  <si>
+    <t>Final presentation</t>
+  </si>
+  <si>
+    <t>Extensive edits to document for meaning, grammar, spelling, citation,data, content, cohesion, etc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -885,38 +895,38 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -924,7 +934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
@@ -935,7 +945,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>5</v>
@@ -944,7 +954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>6</v>
@@ -953,16 +963,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>26</v>
       </c>
@@ -973,7 +983,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" t="s">
         <v>49</v>
@@ -982,7 +992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" t="s">
         <v>48</v>
@@ -991,13 +1001,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
@@ -1008,19 +1018,19 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -1031,19 +1041,19 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>29</v>
       </c>
@@ -1054,16 +1064,16 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
     </row>
   </sheetData>
@@ -1082,6 +1092,268 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="114.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16"/>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="19"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="19"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="16"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A20:A24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
@@ -1090,38 +1362,38 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1129,7 +1401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
@@ -1140,7 +1412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>9</v>
@@ -1149,7 +1421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>10</v>
@@ -1158,7 +1430,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" t="s">
         <v>11</v>
@@ -1167,10 +1439,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>26</v>
       </c>
@@ -1181,7 +1453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="11" t="s">
         <v>45</v>
@@ -1190,7 +1462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" t="s">
         <v>46</v>
@@ -1199,7 +1471,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" t="s">
         <v>47</v>
@@ -1208,10 +1480,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
@@ -1222,7 +1494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" t="s">
         <v>42</v>
@@ -1231,16 +1503,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -1251,7 +1523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="13" t="s">
         <v>61</v>
@@ -1260,17 +1532,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
     </row>
-    <row r="31" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>29</v>
       </c>
@@ -1281,7 +1553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
       <c r="B33" s="9" t="s">
         <v>33</v>
@@ -1290,13 +1562,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
     </row>
   </sheetData>
@@ -1323,38 +1595,38 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1362,7 +1634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>31</v>
       </c>
@@ -1373,7 +1645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>13</v>
@@ -1382,7 +1654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>14</v>
@@ -1391,10 +1663,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -1405,7 +1677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" t="s">
         <v>51</v>
@@ -1414,7 +1686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" t="s">
         <v>52</v>
@@ -1423,7 +1695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" t="s">
         <v>53</v>
@@ -1432,27 +1704,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>28</v>
       </c>
@@ -1463,19 +1735,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>29</v>
       </c>
@@ -1486,16 +1758,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
     </row>
   </sheetData>
@@ -1521,38 +1793,38 @@
       <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1560,7 +1832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
@@ -1571,7 +1843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>16</v>
@@ -1580,7 +1852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>17</v>
@@ -1589,7 +1861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" t="s">
         <v>43</v>
@@ -1598,7 +1870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" t="s">
         <v>30</v>
@@ -1607,10 +1879,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>26</v>
       </c>
@@ -1621,7 +1893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" t="s">
         <v>55</v>
@@ -1630,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" t="s">
         <v>57</v>
@@ -1639,7 +1911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" t="s">
         <v>56</v>
@@ -1648,7 +1920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" t="s">
         <v>58</v>
@@ -1657,7 +1929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" t="s">
         <v>59</v>
@@ -1666,7 +1938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>27</v>
       </c>
@@ -1677,7 +1949,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" t="s">
         <v>37</v>
@@ -1686,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" t="s">
         <v>38</v>
@@ -1695,7 +1967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" t="s">
         <v>39</v>
@@ -1704,10 +1976,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>28</v>
       </c>
@@ -1718,7 +1990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="15" t="s">
         <v>63</v>
@@ -1727,7 +1999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="15" t="s">
         <v>64</v>
@@ -1736,13 +2008,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>29</v>
       </c>
@@ -1753,7 +2025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="B34" t="s">
         <v>34</v>
@@ -1762,7 +2034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
       <c r="B35" t="s">
         <v>35</v>
@@ -1771,7 +2043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
       <c r="B36" t="s">
         <v>36</v>
@@ -1780,7 +2052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
     </row>
   </sheetData>
@@ -1807,38 +2079,38 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1846,7 +2118,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
@@ -1857,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>67</v>
@@ -1866,7 +2138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" t="s">
         <v>68</v>
@@ -1875,10 +2147,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -1889,7 +2161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="16" t="s">
         <v>70</v>
@@ -1898,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="16" t="s">
         <v>71</v>
@@ -1907,7 +2179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="16" t="s">
         <v>72</v>
@@ -1916,7 +2188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="16" t="s">
         <v>79</v>
@@ -1925,7 +2197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>27</v>
       </c>
@@ -1933,7 +2205,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="16" t="s">
         <v>74</v>
@@ -1942,10 +2214,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" t="s">
         <v>72</v>
@@ -1954,10 +2226,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>28</v>
       </c>
@@ -1968,7 +2240,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" t="s">
         <v>77</v>
@@ -1977,7 +2249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" t="s">
         <v>78</v>
@@ -1986,7 +2258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" t="s">
         <v>72</v>
@@ -1995,10 +2267,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>29</v>
       </c>
@@ -2009,7 +2281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" t="s">
         <v>76</v>
@@ -2018,13 +2290,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
     </row>
   </sheetData>
@@ -2050,38 +2322,38 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2089,7 +2361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
@@ -2100,7 +2372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" t="s">
         <v>88</v>
@@ -2109,7 +2381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="16" t="s">
         <v>72</v>
@@ -2118,7 +2390,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" t="s">
         <v>90</v>
@@ -2127,10 +2399,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>26</v>
       </c>
@@ -2141,7 +2413,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="16" t="s">
         <v>80</v>
@@ -2150,7 +2422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="16" t="s">
         <v>85</v>
@@ -2159,7 +2431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="16" t="s">
         <v>82</v>
@@ -2168,7 +2440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="16" t="s">
         <v>81</v>
@@ -2177,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="16" t="s">
         <v>83</v>
@@ -2186,8 +2458,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
@@ -2198,7 +2470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="16" t="s">
         <v>119</v>
@@ -2207,7 +2479,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" t="s">
         <v>121</v>
@@ -2216,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="16" t="s">
         <v>120</v>
@@ -2225,7 +2497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="16" t="s">
         <v>122</v>
@@ -2234,7 +2506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -2245,7 +2517,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" t="s">
         <v>72</v>
@@ -2254,7 +2526,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" t="s">
         <v>87</v>
@@ -2263,13 +2535,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>29</v>
       </c>
@@ -2280,7 +2552,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" t="s">
         <v>91</v>
@@ -2289,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="B34" t="s">
         <v>92</v>
@@ -2298,10 +2570,10 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
     </row>
   </sheetData>
@@ -2328,39 +2600,39 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="16"/>
+    <col min="2" max="2" width="103.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2368,7 +2640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
@@ -2379,7 +2651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="16" t="s">
         <v>99</v>
@@ -2388,7 +2660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="16" t="s">
         <v>100</v>
@@ -2397,13 +2669,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>26</v>
       </c>
@@ -2414,7 +2686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="16" t="s">
         <v>103</v>
@@ -2423,7 +2695,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="16" t="s">
         <v>102</v>
@@ -2432,7 +2704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="16" t="s">
         <v>104</v>
@@ -2441,13 +2713,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
@@ -2458,19 +2730,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -2481,7 +2753,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="16" t="s">
         <v>93</v>
@@ -2490,7 +2762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="16" t="s">
         <v>96</v>
@@ -2499,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="16" t="s">
         <v>97</v>
@@ -2508,10 +2780,10 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>29</v>
       </c>
@@ -2522,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="16" t="s">
         <v>94</v>
@@ -2531,13 +2803,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
     </row>
   </sheetData>
@@ -2564,52 +2836,52 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="99.5" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="99.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C6" s="16"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -2618,7 +2890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
@@ -2629,7 +2901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="16" t="s">
         <v>106</v>
@@ -2638,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="16" t="s">
         <v>66</v>
@@ -2647,7 +2919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="16" t="s">
         <v>107</v>
@@ -2656,12 +2928,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>26</v>
       </c>
@@ -2672,7 +2944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" t="s">
         <v>106</v>
@@ -2681,7 +2953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="16" t="s">
         <v>66</v>
@@ -2690,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="16" t="s">
         <v>107</v>
@@ -2699,22 +2971,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
@@ -2725,32 +2997,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -2761,7 +3033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="16" t="s">
         <v>108</v>
@@ -2770,7 +3042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" t="s">
         <v>72</v>
@@ -2779,22 +3051,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>29</v>
       </c>
@@ -2805,7 +3077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="16" t="s">
         <v>94</v>
@@ -2814,17 +3086,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -2848,43 +3120,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="A1:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="99.5" style="16" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="16" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="16"/>
+    <col min="1" max="1" width="11.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="99.42578125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2892,7 +3164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
@@ -2903,7 +3175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="16" t="s">
         <v>66</v>
@@ -2912,7 +3184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="16" t="s">
         <v>115</v>
@@ -2921,13 +3193,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>26</v>
       </c>
@@ -2938,7 +3210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="16" t="s">
         <v>117</v>
@@ -2947,7 +3219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="16" t="s">
         <v>66</v>
@@ -2956,16 +3228,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
@@ -2976,7 +3248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="16" t="s">
         <v>126</v>
@@ -2985,7 +3257,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="16" t="s">
         <v>127</v>
@@ -2994,7 +3266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="16" t="s">
         <v>128</v>
@@ -3003,10 +3275,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -3017,7 +3289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="16" t="s">
         <v>108</v>
@@ -3026,7 +3298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="16" t="s">
         <v>66</v>
@@ -3035,13 +3307,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>29</v>
       </c>
@@ -3052,7 +3324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="16" t="s">
         <v>94</v>
@@ -3061,13 +3333,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
     </row>
   </sheetData>

</xml_diff>